<commit_message>
Added time settings in solver GUI
</commit_message>
<xml_diff>
--- a/kinematyka5.xlsx
+++ b/kinematyka5.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +799,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>